<commit_message>
Add Save Game Achieve Result
</commit_message>
<xml_diff>
--- a/Assets/8. Execl/AchieveDB.xlsx
+++ b/Assets/8. Execl/AchieveDB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sojun\cosmos\Assets\8. Execl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{611B2974-19EF-4089-8DA2-789BD5C917A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F55E2DAD-0781-4E06-857C-A2E5836D2120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="28800" windowHeight="15345" xr2:uid="{8FD17F28-07B5-4A0D-A0B0-20EFBE75B016}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{8FD17F28-07B5-4A0D-A0B0-20EFBE75B016}"/>
   </bookViews>
   <sheets>
     <sheet name="Achieves" sheetId="1" r:id="rId1"/>
@@ -20,20 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="38">
   <si>
     <t>achieveName</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -51,31 +43,133 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>EnemyA</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Kill Enemy A</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>10,20,30,40</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>EnemyB</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Kill Enemy B</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>50,100,150,200</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>maxAchieveLevel</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Starting from the basic</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Not so fast?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Quite Fragile</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gross. Go Away</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MotherShip Down</t>
+  </si>
+  <si>
+    <t>It was close</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>I’m Not a Sun</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SpaceKing</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>What a good balance</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>World Class Engineer</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Alien? Zombie?</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Kill Monster C</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Kill Monster A</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Kill Monster B</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Kill Monster D</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Kill Stage 10 Boss</t>
+  </si>
+  <si>
+    <t>Kill Stage 20 Boss</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Kill Stage 30 Boss</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>KIll Stage 40 Boss</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>?????????????</t>
+  </si>
+  <si>
+    <t>?????????????</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>StarWars</t>
+  </si>
+  <si>
+    <t>100,150,200,250,300</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>50,75,100,125,150</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>50,80,110,140,170</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>3,8,13,18,22</t>
+  </si>
+  <si>
+    <t>3,8,13,18,22</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>10,20,30,40,50</t>
+  </si>
+  <si>
+    <t>10,20,30,40,50</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>30</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>4</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>50</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>100</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -136,7 +230,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -144,9 +238,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
@@ -467,15 +558,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22E03B99-B5DD-43ED-810B-366F2B568B78}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="16.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.625" customWidth="1"/>
+    <col min="5" max="5" width="32.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -486,7 +581,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -497,36 +592,206 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="3">
         <v>5</v>
       </c>
-      <c r="C2" s="4">
-        <v>4</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="3">
-        <v>4</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>6</v>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>